<commit_message>
New members added to the dataset
</commit_message>
<xml_diff>
--- a/NetworkVisualisationData/EMERGENCECollatedData.xlsx
+++ b/NetworkVisualisationData/EMERGENCECollatedData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d052a0d9fa7cbf49/Documents/psymh9-EMERGENCE-visualisation/NetworkVisualisationData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="8_{5865E62E-5C8A-44C3-B1E8-685C63108DCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76E2A318-0FBA-47A3-A325-6BFC36111182}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{5865E62E-5C8A-44C3-B1E8-685C63108DCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A27F528-6406-4D62-91D8-305DFE8AFA03}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1523" uniqueCount="688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1520" uniqueCount="687">
   <si>
     <t>ID</t>
   </si>
@@ -2128,9 +2128,6 @@
   </si>
   <si>
     <t>Manchester</t>
-  </si>
-  <si>
-    <t>Maximus Hughes-Gray</t>
   </si>
 </sst>
 </file>
@@ -2611,10 +2608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R140"/>
+  <dimension ref="A1:R139"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="F140" sqref="F140"/>
+      <selection activeCell="A140" sqref="A140:XFD140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8601,20 +8598,6 @@
         <v>654</v>
       </c>
     </row>
-    <row r="140" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B140" s="31">
-        <v>44991.607517384255</v>
-      </c>
-      <c r="F140" t="s">
-        <v>687</v>
-      </c>
-      <c r="G140" t="s">
-        <v>63</v>
-      </c>
-      <c r="H140" t="s">
-        <v>672</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="N101" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>